<commit_message>
added educator quality guide
</commit_message>
<xml_diff>
--- a/data/dictionaries/2017_School_Quality_Report_DD.xlsx
+++ b/data/dictionaries/2017_School_Quality_Report_DD.xlsx
@@ -20,7 +20,7 @@
     <definedName name="front_data" localSheetId="1">'Column Info'!#REF!</definedName>
     <definedName name="front_data" localSheetId="2">'Dataset Revision History'!$A$2:$D$2</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -9566,8 +9566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1753"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B112" sqref="B112"/>
+    <sheetView tabSelected="1" topLeftCell="A809" workbookViewId="0">
+      <selection activeCell="D842" sqref="D842"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>